<commit_message>
Make actual predictions for 2022
</commit_message>
<xml_diff>
--- a/source/data/my_data/ncaaGameLocations.xlsx
+++ b/source/data/my_data/ncaaGameLocations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kniu91/Documents/Kevin's Folders/Grad Schools/UChicago MPCS/ncaa/source/data/my_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ABFF40-0FEB-F945-9361-60A88D77E31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D015AFD-931F-0246-84F6-BF66AC6D6861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="14640" xr2:uid="{E7937B0F-1CFD-D447-A089-7E1C9A11171B}"/>
   </bookViews>
@@ -486,9 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73619810-9FD5-8543-A91E-7662C15FE1B8}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>